<commit_message>
mod: haag15/building_to_edge uses geopandas for geographic coord support
</commit_message>
<xml_diff>
--- a/data/haag15/data.xlsx
+++ b/data/haag15/data.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\Projekte\Promotion\Modelle\rivus\data\haag15\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="75" windowWidth="22515" windowHeight="9780" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="600" yWindow="75" windowWidth="22515" windowHeight="9780" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Readme" sheetId="6" r:id="rId1"/>
@@ -14,7 +19,7 @@
     <sheet name="Time" sheetId="5" r:id="rId5"/>
     <sheet name="Area-Demand" sheetId="3" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -569,7 +574,7 @@
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="11">
+  <dxfs count="14">
     <dxf>
       <border>
         <top style="thin">
@@ -582,6 +587,11 @@
     <dxf>
       <font>
         <color theme="5" tint="0.59996337778862885"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="6" tint="0.59996337778862885"/>
       </font>
     </dxf>
     <dxf>
@@ -605,13 +615,9 @@
       </font>
     </dxf>
     <dxf>
-      <border>
-        <top style="thin">
-          <color theme="0" tint="-0.499984740745262"/>
-        </top>
-        <vertical/>
-        <horizontal/>
-      </border>
+      <font>
+        <color theme="6" tint="0.59996337778862885"/>
+      </font>
     </dxf>
     <dxf>
       <border>
@@ -623,13 +629,15 @@
       </border>
     </dxf>
     <dxf>
-      <border>
-        <top style="thin">
-          <color theme="0" tint="-0.499984740745262"/>
-        </top>
-        <vertical/>
-        <horizontal/>
-      </border>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="6" tint="0.59996337778862885"/>
+      </font>
     </dxf>
     <dxf>
       <border>
@@ -641,13 +649,10 @@
       </border>
     </dxf>
     <dxf>
-      <border>
-        <top style="thin">
-          <color theme="0" tint="-0.499984740745262"/>
-        </top>
-        <vertical/>
-        <horizontal/>
-      </border>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
     </dxf>
     <dxf>
       <border>
@@ -658,20 +663,29 @@
         <horizontal/>
       </border>
     </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Larissa">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -709,9 +723,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Larissa">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -746,7 +760,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -781,7 +795,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Larissa">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1314,7 +1328,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -1488,7 +1502,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="containsErrors" dxfId="4" priority="1">
+    <cfRule type="containsErrors" dxfId="5" priority="1">
       <formula>ISERROR(A1)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1704,11 +1718,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A8" sqref="A8"/>
+      <selection pane="bottomRight" activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1973,7 +1987,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="dataBar" priority="3">
+    <cfRule type="dataBar" priority="4">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="num" val="2"/>
@@ -1987,15 +2001,20 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="expression" dxfId="3" priority="1">
-      <formula>EXACT("In", INDIRECT("Z"&amp;ROW()&amp;"S3",FALSE()))</formula>
+    <cfRule type="expression" dxfId="4" priority="2">
+      <formula>NOT(EXACT(INDIRECT("Z"&amp;(ROW()-1)&amp;"S1",FALSE()),INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="2">
+    <cfRule type="expression" dxfId="3" priority="3">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="A2:A1000">
+    <cfRule type="expression" dxfId="2" priority="1">
+      <formula>EXACT(INDIRECT("Z"&amp;(ROW()-1)&amp;"S1",FALSE()),INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE()))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Input/output ratio (kWh/kWh)" prompt="Relative power flows in and out of processes. Sum of In and sum of Out should be equal to 1._x000a_For CO2, unit is kg/kWh." sqref="D1"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Input/output ratio" prompt="Flows in and out of processes, relative to 1 unit of throughput. For CO2, unit is kg/kWh (for example)" sqref="D1"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2029,7 +2048,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="B6" sqref="B6:D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2110,7 +2129,7 @@
         <v>0.25</v>
       </c>
       <c r="D5" s="8">
-        <v>0.17</v>
+        <v>0.1</v>
       </c>
       <c r="F5" s="35"/>
     </row>
@@ -2137,7 +2156,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C25" sqref="C25"/>
+      <selection pane="bottomRight" activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
haag15/data.xlsx: elec more expensive, gas cheaper
</commit_message>
<xml_diff>
--- a/data/haag15/data.xlsx
+++ b/data/haag15/data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jdorfner\Documents\Themen\Thesis\Modelle\rivus\data\haag15\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\Projekte\Promotion\Modelle\rivus\data\haag15\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1293,7 +1293,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H25" sqref="H25"/>
+      <selection pane="bottomRight" activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1356,7 +1356,7 @@
         <v>7</v>
       </c>
       <c r="F2" s="37">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
       <c r="G2" s="10">
         <v>1E-3</v>
@@ -1389,7 +1389,7 @@
         <v>5</v>
       </c>
       <c r="F3" s="37">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="G3" s="10">
         <v>1E-4</v>

</xml_diff>

<commit_message>
more scenarios, cluster labels in map
</commit_message>
<xml_diff>
--- a/data/haag15/data.xlsx
+++ b/data/haag15/data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="75" windowWidth="22515" windowHeight="9780" activeTab="1"/>
+    <workbookView xWindow="600" yWindow="75" windowWidth="22515" windowHeight="9780" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Readme" sheetId="6" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="80">
   <si>
     <t>Commodity</t>
   </si>
@@ -93,9 +93,6 @@
   </si>
   <si>
     <t>loss-var</t>
-  </si>
-  <si>
-    <t>CAPMIN</t>
   </si>
   <si>
     <t>- Commodity</t>
@@ -231,9 +228,6 @@
     </r>
   </si>
   <si>
-    <t>Linear mixed-integer optimization model for urban energy infrastructure</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">area, type, nearest edge ID: is aggregated to </t>
     </r>
@@ -344,6 +338,12 @@
   </si>
   <si>
     <t>cost-fix</t>
+  </si>
+  <si>
+    <t>rivus</t>
+  </si>
+  <si>
+    <t>Input file for haag15 dataset</t>
   </si>
 </sst>
 </file>
@@ -933,7 +933,7 @@
   <dimension ref="B2:J28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -956,7 +956,7 @@
     <row r="3" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B3" s="16"/>
       <c r="C3" s="17" t="s">
-        <v>23</v>
+        <v>78</v>
       </c>
       <c r="D3" s="18"/>
       <c r="E3" s="18"/>
@@ -969,7 +969,7 @@
     <row r="4" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B4" s="16"/>
       <c r="C4" s="20" t="s">
-        <v>46</v>
+        <v>79</v>
       </c>
       <c r="D4" s="18"/>
       <c r="E4" s="18"/>
@@ -1004,7 +1004,7 @@
     <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7" s="21"/>
       <c r="C7" s="30" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D7" s="12"/>
       <c r="E7" s="12"/>
@@ -1017,11 +1017,11 @@
     <row r="8" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B8" s="21"/>
       <c r="C8" s="28" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D8" s="12"/>
       <c r="E8" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F8" s="12"/>
       <c r="G8" s="12"/>
@@ -1032,11 +1032,11 @@
     <row r="9" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B9" s="21"/>
       <c r="C9" s="28" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D9" s="12"/>
       <c r="E9" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F9" s="12"/>
       <c r="G9" s="12"/>
@@ -1047,11 +1047,11 @@
     <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B10" s="21"/>
       <c r="C10" s="29" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D10" s="12"/>
       <c r="E10" s="12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F10" s="12"/>
       <c r="G10" s="12"/>
@@ -1062,11 +1062,11 @@
     <row r="11" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B11" s="21"/>
       <c r="C11" s="28" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D11" s="12"/>
       <c r="E11" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F11" s="12"/>
       <c r="G11" s="12"/>
@@ -1077,11 +1077,11 @@
     <row r="12" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B12" s="21"/>
       <c r="C12" s="28" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D12" s="12"/>
       <c r="E12" s="12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F12" s="12"/>
       <c r="G12" s="12"/>
@@ -1103,7 +1103,7 @@
     <row r="14" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B14" s="21"/>
       <c r="C14" s="30" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D14" s="12"/>
       <c r="E14" s="12"/>
@@ -1116,11 +1116,11 @@
     <row r="15" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B15" s="21"/>
       <c r="C15" s="28" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D15" s="12"/>
       <c r="E15" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F15" s="12"/>
       <c r="G15" s="12"/>
@@ -1131,11 +1131,11 @@
     <row r="16" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B16" s="21"/>
       <c r="C16" s="28" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D16" s="12"/>
       <c r="E16" s="12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F16" s="12"/>
       <c r="G16" s="12"/>
@@ -1146,11 +1146,11 @@
     <row r="17" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B17" s="21"/>
       <c r="C17" s="28" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D17" s="12"/>
       <c r="E17" s="12" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F17" s="12"/>
       <c r="G17" s="12"/>
@@ -1289,11 +1289,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F3" sqref="F3"/>
+      <selection pane="bottomRight" activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1321,7 +1321,7 @@
         <v>15</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F1" s="5" t="s">
         <v>8</v>
@@ -1336,7 +1336,7 @@
         <v>17</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -1347,19 +1347,19 @@
         <v>5</v>
       </c>
       <c r="C2" s="3">
-        <v>250</v>
+        <v>300</v>
       </c>
       <c r="D2" s="3">
-        <v>4.0000000000000003E-5</v>
+        <v>2.0000000000000002E-5</v>
       </c>
       <c r="E2" s="3">
         <v>7</v>
       </c>
       <c r="F2" s="37">
-        <v>0.03</v>
+        <v>0.01</v>
       </c>
       <c r="G2" s="10">
-        <v>1E-3</v>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="H2" s="10">
         <v>0</v>
@@ -1380,7 +1380,7 @@
         <v>5</v>
       </c>
       <c r="C3" s="3">
-        <v>100</v>
+        <v>175</v>
       </c>
       <c r="D3" s="3">
         <v>1.0000000000000001E-5</v>
@@ -1392,7 +1392,7 @@
         <v>0.3</v>
       </c>
       <c r="G3" s="10">
-        <v>1E-4</v>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="H3" s="10">
         <v>0</v>
@@ -1413,20 +1413,20 @@
         <v>5</v>
       </c>
       <c r="C4" s="3">
-        <v>500</v>
+        <v>350</v>
       </c>
       <c r="D4" s="3">
-        <v>2.0000000000000001E-4</v>
+        <v>1E-4</v>
       </c>
       <c r="E4" s="3">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F4" s="38" t="e">
         <f>NA()</f>
         <v>#N/A</v>
       </c>
       <c r="G4" s="10">
-        <v>2E-3</v>
+        <v>2.0000000000000001E-4</v>
       </c>
       <c r="H4" s="10">
         <v>2.0000000000000002E-5</v>
@@ -1475,7 +1475,7 @@
         <v>#N/A</v>
       </c>
       <c r="J5" s="31" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -1503,11 +1503,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E8" sqref="E8"/>
+      <selection pane="bottomRight" activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1516,7 +1516,7 @@
     <col min="2" max="2" width="11.42578125" style="35"/>
     <col min="3" max="3" width="11.42578125" style="3"/>
     <col min="4" max="4" width="11.42578125" style="40"/>
-    <col min="5" max="5" width="11.42578125" style="3"/>
+    <col min="5" max="5" width="11.42578125" style="27"/>
     <col min="6" max="7" width="11.42578125" style="35"/>
     <col min="8" max="16384" width="11.42578125" style="3"/>
   </cols>
@@ -1532,9 +1532,9 @@
         <v>15</v>
       </c>
       <c r="D1" s="39" t="s">
-        <v>79</v>
-      </c>
-      <c r="E1" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E1" s="26" t="s">
         <v>8</v>
       </c>
       <c r="F1" s="34" t="s">
@@ -1544,49 +1544,49 @@
         <v>17</v>
       </c>
       <c r="I1" s="36" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B2" s="35">
         <v>20000</v>
       </c>
       <c r="C2" s="3">
-        <v>1000</v>
+        <v>100</v>
       </c>
       <c r="D2" s="40">
         <v>50</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="27">
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="F2" s="35">
-        <v>15000</v>
+        <v>10000</v>
       </c>
       <c r="G2" s="35">
         <v>600000</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B3" s="35">
         <v>0</v>
       </c>
       <c r="C3" s="3">
-        <v>2500</v>
+        <v>250</v>
       </c>
       <c r="D3" s="40">
         <v>30</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="27">
         <v>0.1</v>
       </c>
       <c r="F3" s="35">
@@ -1596,24 +1596,24 @@
         <v>50000</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B4" s="35">
         <v>25000</v>
       </c>
       <c r="C4" s="3">
-        <v>1800</v>
+        <v>180</v>
       </c>
       <c r="D4" s="40">
         <v>75</v>
       </c>
-      <c r="E4" s="3">
-        <v>1.2999999999999999E-2</v>
+      <c r="E4" s="27">
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="F4" s="35">
         <v>10000</v>
@@ -1622,24 +1622,24 @@
         <v>150000</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B5" s="35">
         <v>0</v>
       </c>
       <c r="C5" s="3">
-        <v>2800</v>
+        <v>250</v>
       </c>
       <c r="D5" s="40">
         <v>100</v>
       </c>
-      <c r="E5" s="3">
-        <v>2.5000000000000001E-2</v>
+      <c r="E5" s="27">
+        <v>0.1</v>
       </c>
       <c r="F5" s="35">
         <v>0</v>
@@ -1650,18 +1650,18 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B6" s="35">
         <v>30000</v>
       </c>
       <c r="C6" s="3">
-        <v>600</v>
+        <v>60</v>
       </c>
       <c r="D6" s="40">
         <v>60</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="27">
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="F6" s="35">
@@ -1671,23 +1671,23 @@
         <v>500000</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B7" s="35">
         <v>25000</v>
       </c>
       <c r="C7" s="3">
-        <v>1500</v>
+        <v>150</v>
       </c>
       <c r="D7" s="40">
         <v>50</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="27">
         <v>2.7E-2</v>
       </c>
       <c r="F7" s="35">
@@ -1697,23 +1697,23 @@
         <v>350000</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B8" s="35">
         <v>0</v>
       </c>
       <c r="C8" s="3">
-        <v>1700</v>
+        <v>40</v>
       </c>
       <c r="D8" s="40">
-        <v>80</v>
-      </c>
-      <c r="E8" s="3">
+        <v>40</v>
+      </c>
+      <c r="E8" s="27">
         <f>0.023</f>
         <v>2.3E-2</v>
       </c>
@@ -1724,7 +1724,7 @@
         <v>50000</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -1743,13 +1743,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D10" sqref="D10"/>
+      <selection pane="bottomRight" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1776,7 +1776,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>1</v>
@@ -1790,7 +1790,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>2</v>
@@ -1804,7 +1804,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>3</v>
@@ -1818,7 +1818,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>6</v>
@@ -1832,7 +1832,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>2</v>
@@ -1846,7 +1846,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>3</v>
@@ -1855,71 +1855,71 @@
         <v>12</v>
       </c>
       <c r="D7" s="8">
-        <v>1.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>48</v>
+        <v>70</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D8" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D9" s="8">
-        <v>0.99</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>78</v>
+        <v>46</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D10" s="8">
-        <v>1</v>
+        <v>0.99</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>78</v>
+        <v>46</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D11" s="8">
-        <v>1.3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>50</v>
+        <v>76</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>11</v>
@@ -1930,21 +1930,21 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>50</v>
+        <v>76</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D13" s="8">
-        <v>0.35</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>50</v>
+        <v>76</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>6</v>
@@ -1953,12 +1953,12 @@
         <v>12</v>
       </c>
       <c r="D14" s="8">
-        <v>0.02</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>1</v>
@@ -1972,21 +1972,21 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D16" s="8">
-        <v>0.98</v>
+        <v>0.35</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>6</v>
@@ -2000,7 +2000,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>1</v>
@@ -2014,7 +2014,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>3</v>
@@ -2023,12 +2023,12 @@
         <v>12</v>
       </c>
       <c r="D19" s="8">
-        <v>0.95</v>
+        <v>0.98</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>6</v>
@@ -2037,6 +2037,48 @@
         <v>12</v>
       </c>
       <c r="D20" s="8">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D21" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D22" s="8">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D23" s="8">
         <v>0.03</v>
       </c>
     </row>
@@ -2063,7 +2105,7 @@
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:A1002">
+  <conditionalFormatting sqref="A2:A1005">
     <cfRule type="expression" dxfId="2" priority="1">
       <formula>EXACT(INDIRECT("Z"&amp;(ROW()-1)&amp;"S1",FALSE()),INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE()))</formula>
     </cfRule>
@@ -2130,7 +2172,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B2" s="35">
         <v>3055</v>
@@ -2145,7 +2187,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B3" s="35">
         <v>3708</v>
@@ -2160,7 +2202,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B4" s="35">
         <v>1339</v>
@@ -2175,7 +2217,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B5" s="35">
         <v>508</v>
@@ -2190,7 +2232,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B6" s="35">
         <v>150</v>
@@ -2234,7 +2276,7 @@
   <sheetData>
     <row r="1" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>0</v>
@@ -2245,7 +2287,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>2</v>
@@ -2256,7 +2298,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>3</v>
@@ -2267,7 +2309,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>2</v>
@@ -2278,7 +2320,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>3</v>
@@ -2289,7 +2331,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>2</v>
@@ -2300,7 +2342,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>3</v>
@@ -2311,7 +2353,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>2</v>
@@ -2322,7 +2364,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>3</v>
@@ -2333,7 +2375,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>2</v>
@@ -2344,7 +2386,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>3</v>
@@ -2355,7 +2397,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>2</v>
@@ -2366,7 +2408,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>3</v>
@@ -2377,7 +2419,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>2</v>
@@ -2388,7 +2430,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>3</v>
@@ -2399,7 +2441,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>2</v>
@@ -2410,7 +2452,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>3</v>
@@ -2421,7 +2463,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>2</v>
@@ -2432,7 +2474,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>3</v>
@@ -2443,7 +2485,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>2</v>
@@ -2454,7 +2496,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>3</v>
@@ -2465,7 +2507,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>2</v>
@@ -2476,7 +2518,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>3</v>
@@ -2487,7 +2529,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>2</v>
@@ -2498,7 +2540,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>3</v>
@@ -2509,7 +2551,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>2</v>
@@ -2520,7 +2562,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>3</v>
@@ -2531,7 +2573,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>2</v>
@@ -2542,7 +2584,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>3</v>
@@ -2553,7 +2595,7 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>2</v>
@@ -2564,7 +2606,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
added house, commercial, office to renovation scenario; warehouse area_demand added
</commit_message>
<xml_diff>
--- a/data/haag15/data.xlsx
+++ b/data/haag15/data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="75" windowWidth="22515" windowHeight="9780" activeTab="2"/>
+    <workbookView xWindow="600" yWindow="75" windowWidth="22515" windowHeight="9780" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Readme" sheetId="6" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="81">
   <si>
     <t>Commodity</t>
   </si>
@@ -344,6 +344,9 @@
   </si>
   <si>
     <t>Input file for haag15 dataset</t>
+  </si>
+  <si>
+    <t>warehouse</t>
   </si>
 </sst>
 </file>
@@ -1293,7 +1296,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E30" sqref="E30"/>
+      <selection pane="bottomRight" activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1380,7 +1383,7 @@
         <v>5</v>
       </c>
       <c r="C3" s="3">
-        <v>175</v>
+        <v>275</v>
       </c>
       <c r="D3" s="3">
         <v>1.0000000000000001E-5</v>
@@ -1503,7 +1506,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -2257,13 +2260,13 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C31"/>
+  <dimension ref="A1:C33"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D22" sqref="D22"/>
+      <selection pane="bottomRight" activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2595,23 +2598,45 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C30" s="27">
-        <v>0</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C31" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C32" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C33" s="27">
         <v>0</v>
       </c>
     </row>

</xml_diff>